<commit_message>
Added row for notes
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E86CAC-91DE-4945-80DB-0545FDA49EC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2385D51E-71A1-4D4B-BC6E-4680E84FCE1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
+    <workbookView xWindow="0" yWindow="1230" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="400">
   <si>
     <t>course_code</t>
   </si>
@@ -106,9 +106,6 @@
     <t>MATH 1620</t>
   </si>
   <si>
-    <t>MATH 750</t>
-  </si>
-  <si>
     <t>MATH 0060</t>
   </si>
   <si>
@@ -1232,6 +1229,9 @@
   </si>
   <si>
     <t>La question animale</t>
+  </si>
+  <si>
+    <t>The year-long sequence of Math 0750/ Math 0760 may be substituted for one 1000-level Math Course. Selecting Math 0750 will add it and Math 0760 to your requirements</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FF0174-35EF-4838-880B-C4F8D4E4CC9D}">
   <dimension ref="A2:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
@@ -1616,265 +1616,265 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P2" t="s">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="P4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1882,75 +1882,75 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1958,37 +1958,37 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1996,75 +1996,75 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2072,37 +2072,37 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2110,113 +2110,113 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Q17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2224,37 +2224,37 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2262,37 +2262,37 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2300,37 +2300,37 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2338,37 +2338,37 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2376,37 +2376,37 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2414,37 +2414,37 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2452,31 +2452,31 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2484,31 +2484,31 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -2516,31 +2516,31 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -2548,31 +2548,31 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -2580,31 +2580,31 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P28" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2612,19 +2612,19 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2632,19 +2632,19 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -2652,19 +2652,19 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -2672,19 +2672,19 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2692,19 +2692,19 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2712,165 +2712,165 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N43" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2883,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AC56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,72 +2901,75 @@
   <sheetData>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="V2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
       <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
         <v>72</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>333</v>
+      </c>
+      <c r="M3" t="s">
+        <v>334</v>
+      </c>
+      <c r="N3" t="s">
+        <v>335</v>
+      </c>
+      <c r="O3" t="s">
+        <v>336</v>
+      </c>
+      <c r="P3" t="s">
+        <v>337</v>
+      </c>
+      <c r="V3" t="s">
         <v>73</v>
       </c>
-      <c r="L3" t="s">
-        <v>334</v>
-      </c>
-      <c r="M3" t="s">
-        <v>335</v>
-      </c>
-      <c r="N3" t="s">
-        <v>336</v>
-      </c>
-      <c r="O3" t="s">
-        <v>337</v>
-      </c>
-      <c r="P3" t="s">
-        <v>338</v>
-      </c>
-      <c r="V3" t="s">
-        <v>74</v>
-      </c>
       <c r="W3" t="s">
+        <v>340</v>
+      </c>
+      <c r="X3" t="s">
         <v>341</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>342</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>343</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>344</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>345</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>346</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -3048,43 +3051,43 @@
         <v>6</v>
       </c>
       <c r="L5" t="s">
+        <v>155</v>
+      </c>
+      <c r="M5" t="s">
         <v>156</v>
       </c>
-      <c r="M5" t="s">
-        <v>157</v>
-      </c>
       <c r="N5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="V5" t="s">
         <v>8</v>
       </c>
       <c r="W5" t="s">
+        <v>250</v>
+      </c>
+      <c r="X5" t="s">
         <v>251</v>
       </c>
-      <c r="X5" t="s">
-        <v>252</v>
-      </c>
       <c r="Y5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AA5" t="s">
         <v>9</v>
       </c>
       <c r="AB5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AC5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -3104,28 +3107,28 @@
         <v>7</v>
       </c>
       <c r="N6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="W6" t="s">
+        <v>252</v>
+      </c>
+      <c r="X6" t="s">
         <v>253</v>
       </c>
-      <c r="X6" t="s">
-        <v>254</v>
-      </c>
       <c r="Y6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA6" t="s">
         <v>10</v>
       </c>
       <c r="AB6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -3139,22 +3142,22 @@
         <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="X7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AA7" t="s">
         <v>11</v>
       </c>
       <c r="AB7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -3162,16 +3165,16 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AA8" t="s">
         <v>12</v>
       </c>
       <c r="AB8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -3179,13 +3182,13 @@
         <v>13</v>
       </c>
       <c r="O9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA9" t="s">
         <v>13</v>
       </c>
       <c r="AB9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -3193,13 +3196,13 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA10" t="s">
         <v>14</v>
       </c>
       <c r="AB10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -3207,13 +3210,13 @@
         <v>2</v>
       </c>
       <c r="O11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA11" t="s">
         <v>2</v>
       </c>
       <c r="AB11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -3221,13 +3224,13 @@
         <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AA12" t="s">
         <v>15</v>
       </c>
       <c r="AB12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -3235,13 +3238,13 @@
         <v>17</v>
       </c>
       <c r="O13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA13" t="s">
         <v>17</v>
       </c>
       <c r="AB13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -3249,13 +3252,13 @@
         <v>16</v>
       </c>
       <c r="O14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AA14" t="s">
         <v>16</v>
       </c>
       <c r="AB14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -3263,13 +3266,13 @@
         <v>18</v>
       </c>
       <c r="O15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AA15" t="s">
         <v>18</v>
       </c>
       <c r="AB15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -3277,13 +3280,13 @@
         <v>19</v>
       </c>
       <c r="O16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AA16" t="s">
         <v>19</v>
       </c>
       <c r="AB16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -3291,13 +3294,13 @@
         <v>20</v>
       </c>
       <c r="O17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA17" t="s">
         <v>20</v>
       </c>
       <c r="AB17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -3305,13 +3308,13 @@
         <v>21</v>
       </c>
       <c r="O18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA18" t="s">
         <v>21</v>
       </c>
       <c r="AB18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -3319,13 +3322,13 @@
         <v>22</v>
       </c>
       <c r="O19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AA19" t="s">
         <v>22</v>
       </c>
       <c r="AB19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -3336,69 +3339,69 @@
         <v>23</v>
       </c>
       <c r="AB20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="AB21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>79</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>80</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>81</v>
       </c>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
       <c r="AB27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -3424,198 +3427,198 @@
         <v>5</v>
       </c>
       <c r="AB28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
       <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
         <v>40</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>41</v>
       </c>
-      <c r="F29" t="s">
-        <v>42</v>
-      </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AB32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Had to specify shinyjs::, Flex Course
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FC91D6-95BA-45D2-B876-6D4ECE97FE0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB0C6F-1B1A-4AE5-9C5E-25B5AF2C92F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="467">
   <si>
     <t>course_code</t>
   </si>
@@ -1046,9 +1046,6 @@
   </si>
   <si>
     <t>One couse to be approved</t>
-  </si>
-  <si>
-    <t>FLEX 0000</t>
   </si>
   <si>
     <t>math-cs SCB</t>
@@ -1798,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FF0174-35EF-4838-880B-C4F8D4E4CC9D}">
   <dimension ref="A2:U47"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1933,19 +1930,19 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="T3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1998,19 +1995,19 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="T4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -2063,19 +2060,19 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="T5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -2128,19 +2125,19 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="T6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -2193,19 +2190,19 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="T7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -2258,19 +2255,19 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -2323,19 +2320,19 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -2388,19 +2385,19 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -2453,19 +2450,19 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -2518,19 +2515,19 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -2583,19 +2580,19 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2648,19 +2645,19 @@
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="T14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2713,19 +2710,19 @@
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="T15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -2778,19 +2775,19 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -2843,19 +2840,19 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -2908,19 +2905,19 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="T18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -2973,19 +2970,19 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Q19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="T19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -3038,19 +3035,19 @@
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -3103,19 +3100,19 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T21" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -3168,19 +3165,19 @@
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T22" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -3233,19 +3230,19 @@
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -3289,19 +3286,19 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -3345,19 +3342,19 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T25" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -3401,19 +3398,19 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -3457,19 +3454,19 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="T27" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -3513,19 +3510,19 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -3560,10 +3557,10 @@
         <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="T29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3598,10 +3595,10 @@
         <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T30" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="U30">
         <v>0</v>
@@ -3636,10 +3633,10 @@
         <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="T31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -3674,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T32" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -3712,10 +3709,10 @@
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="T33" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="U33">
         <v>0</v>
@@ -3750,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="T34" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -3978,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,22 +3993,22 @@
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K2" t="s">
         <v>332</v>
       </c>
       <c r="V2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -4052,28 +4049,28 @@
         <v>73</v>
       </c>
       <c r="W3" t="s">
+        <v>339</v>
+      </c>
+      <c r="X3" t="s">
         <v>340</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>341</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>342</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>343</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>344</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
+        <v>403</v>
+      </c>
+      <c r="AD3" t="s">
         <v>345</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>404</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -4170,7 +4167,7 @@
         <v>158</v>
       </c>
       <c r="P5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="V5" t="s">
         <v>8</v>
@@ -4194,10 +4191,10 @@
         <v>259</v>
       </c>
       <c r="AC5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AD5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -4247,7 +4244,7 @@
         <v>260</v>
       </c>
       <c r="AC6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -4270,7 +4267,7 @@
         <v>254</v>
       </c>
       <c r="X7" t="s">
-        <v>338</v>
+        <v>399</v>
       </c>
       <c r="AA7" t="s">
         <v>11</v>
@@ -4279,7 +4276,7 @@
         <v>261</v>
       </c>
       <c r="AC7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -4494,7 +4491,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Show course name next to code for major choices
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB0C6F-1B1A-4AE5-9C5E-25B5AF2C92F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE922F-3827-4A31-840C-0935DD72D4EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="468">
   <si>
     <t>course_code</t>
   </si>
@@ -415,18 +415,9 @@
     <t>Analytic Geometry and Calculus</t>
   </si>
   <si>
-    <t xml:space="preserve"> Calculus with Applications to Social Science</t>
-  </si>
-  <si>
     <t>Introductory Calculus, Part I</t>
   </si>
   <si>
-    <t xml:space="preserve"> Introductory Calculus, Part II</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Intermediate Calculus</t>
-  </si>
-  <si>
     <t>Advanced Placement Calculus (Physics/Engineering)</t>
   </si>
   <si>
@@ -1237,9 +1228,6 @@
     <t>APMA 0330 and APMA 0340 will sometimes be accepted in place of APMA 0350 and APMA 0360</t>
   </si>
   <si>
-    <t>Capstone</t>
-  </si>
-  <si>
     <t>Two 1000-level and one intermediate CS courses must satisfy a CS pathway. Check concentrations for more info.</t>
   </si>
   <si>
@@ -1433,6 +1421,21 @@
   </si>
   <si>
     <t>Rhythm and Silence: A Creative Writing Workshop</t>
+  </si>
+  <si>
+    <t>Calculus with Applications to Social Science</t>
+  </si>
+  <si>
+    <t>Introductory Calculus, Part II</t>
+  </si>
+  <si>
+    <t>Intermediate Calculus</t>
+  </si>
+  <si>
+    <t>FlexCourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capstone </t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1799,7 @@
   <dimension ref="A2:U47"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,46 +1906,46 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="Q3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="T3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1968,46 +1971,46 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q4" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="T4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -2018,7 +2021,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>463</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2033,46 +2036,46 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="Q5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="T5" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -2083,7 +2086,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2098,46 +2101,46 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="N6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="Q6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="T6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -2148,7 +2151,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>464</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2163,46 +2166,46 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="Q7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="T7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -2228,46 +2231,46 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="Q8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="T8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -2278,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>465</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2293,46 +2296,46 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="Q9" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="T9" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -2343,7 +2346,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2358,46 +2361,46 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="Q10" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="T10" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -2408,7 +2411,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2423,46 +2426,46 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="Q11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="T11" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -2473,7 +2476,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2488,46 +2491,46 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="Q12" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="T12" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -2538,7 +2541,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2553,46 +2556,46 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="Q13" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="T13" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2618,46 +2621,46 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="N14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="Q14" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="T14" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2668,7 +2671,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2683,46 +2686,46 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N15" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Q15" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="T15" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -2733,7 +2736,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2748,46 +2751,46 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K16" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="N16" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="Q16" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="T16" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -2798,7 +2801,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2813,46 +2816,46 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="N17" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="Q17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="T17" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -2863,7 +2866,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2878,46 +2881,46 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="N18" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="Q18" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="T18" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -2928,7 +2931,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2943,46 +2946,46 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="N19" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="Q19" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="T19" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -2993,7 +2996,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3008,46 +3011,46 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="N20" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="Q20" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="T20" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -3058,7 +3061,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3073,46 +3076,46 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="N21" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="Q21" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="T21" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -3123,7 +3126,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -3138,46 +3141,46 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K22" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="Q22" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="T22" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -3188,7 +3191,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3203,46 +3206,46 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H23" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K23" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N23" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="Q23" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="T23" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -3253,7 +3256,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3268,37 +3271,37 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K24" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N24" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="Q24" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="T24" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -3309,7 +3312,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3324,37 +3327,37 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K25" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N25" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="Q25" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="T25" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -3365,7 +3368,7 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3380,37 +3383,37 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K26" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="N26" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="Q26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="T26" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -3421,7 +3424,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -3436,37 +3439,37 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K27" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N27" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="Q27" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="T27" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -3477,7 +3480,7 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3492,37 +3495,37 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K28" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="N28" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="Q28" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="T28" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -3548,19 +3551,19 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="N29" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="T29" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3571,7 +3574,7 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -3586,19 +3589,19 @@
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="N30" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="T30" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="U30">
         <v>0</v>
@@ -3609,7 +3612,7 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -3624,19 +3627,19 @@
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="N31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="T31" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -3647,7 +3650,7 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -3662,19 +3665,19 @@
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="N32" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="T32" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -3685,7 +3688,7 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -3700,19 +3703,19 @@
         <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="N33" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="T33" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="U33">
         <v>0</v>
@@ -3723,7 +3726,7 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3738,19 +3741,19 @@
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="N34" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="T34" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -3767,10 +3770,10 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="N35" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -3790,10 +3793,10 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N36" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -3810,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N37" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -3830,10 +3833,10 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="N38" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -3850,10 +3853,10 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -3870,10 +3873,10 @@
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N40" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -3890,10 +3893,10 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="N41" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -3901,10 +3904,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="N42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -3912,10 +3915,10 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="N43" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -3923,10 +3926,10 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="N44" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -3934,10 +3937,10 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="N45" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -3945,10 +3948,10 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N46" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -3956,10 +3959,10 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N47" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -3975,8 +3978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,22 +3996,22 @@
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="K2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="V2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="W2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -4031,46 +4034,46 @@
         <v>72</v>
       </c>
       <c r="L3" t="s">
+        <v>330</v>
+      </c>
+      <c r="M3" t="s">
+        <v>331</v>
+      </c>
+      <c r="N3" t="s">
+        <v>332</v>
+      </c>
+      <c r="O3" t="s">
         <v>333</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>334</v>
-      </c>
-      <c r="N3" t="s">
-        <v>335</v>
-      </c>
-      <c r="O3" t="s">
-        <v>336</v>
-      </c>
-      <c r="P3" t="s">
-        <v>337</v>
       </c>
       <c r="V3" t="s">
         <v>73</v>
       </c>
       <c r="W3" t="s">
+        <v>336</v>
+      </c>
+      <c r="X3" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z3" t="s">
         <v>339</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>340</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
         <v>341</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
+        <v>399</v>
+      </c>
+      <c r="AD3" t="s">
         <v>342</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>343</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>344</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>403</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -4155,46 +4158,46 @@
         <v>6</v>
       </c>
       <c r="L5" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" t="s">
+        <v>153</v>
+      </c>
+      <c r="N5" t="s">
+        <v>149</v>
+      </c>
+      <c r="O5" t="s">
         <v>155</v>
       </c>
-      <c r="M5" t="s">
-        <v>156</v>
-      </c>
-      <c r="N5" t="s">
-        <v>152</v>
-      </c>
-      <c r="O5" t="s">
-        <v>158</v>
-      </c>
       <c r="P5" t="s">
-        <v>399</v>
+        <v>466</v>
       </c>
       <c r="V5" t="s">
         <v>8</v>
       </c>
       <c r="W5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="Z5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AA5" t="s">
         <v>9</v>
       </c>
       <c r="AB5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="AC5" t="s">
-        <v>399</v>
+        <v>466</v>
       </c>
       <c r="AD5" t="s">
-        <v>401</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -4214,37 +4217,37 @@
         <v>7</v>
       </c>
       <c r="L6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="W6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="X6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="Y6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Z6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="AA6" t="s">
         <v>10</v>
       </c>
       <c r="AB6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="AC6" t="s">
-        <v>399</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -4258,25 +4261,25 @@
         <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="O7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="W7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="X7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="AA7" t="s">
         <v>11</v>
       </c>
       <c r="AB7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AC7" t="s">
-        <v>399</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -4284,16 +4287,16 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AA8" t="s">
         <v>12</v>
       </c>
       <c r="AB8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -4301,13 +4304,13 @@
         <v>13</v>
       </c>
       <c r="O9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AA9" t="s">
         <v>13</v>
       </c>
       <c r="AB9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -4315,13 +4318,13 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AA10" t="s">
         <v>14</v>
       </c>
       <c r="AB10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -4329,13 +4332,13 @@
         <v>2</v>
       </c>
       <c r="O11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AA11" t="s">
         <v>2</v>
       </c>
       <c r="AB11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -4343,13 +4346,13 @@
         <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AA12" t="s">
         <v>15</v>
       </c>
       <c r="AB12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -4357,13 +4360,13 @@
         <v>17</v>
       </c>
       <c r="O13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AA13" t="s">
         <v>17</v>
       </c>
       <c r="AB13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -4371,13 +4374,13 @@
         <v>16</v>
       </c>
       <c r="O14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AA14" t="s">
         <v>16</v>
       </c>
       <c r="AB14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -4385,13 +4388,13 @@
         <v>18</v>
       </c>
       <c r="O15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AA15" t="s">
         <v>18</v>
       </c>
       <c r="AB15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -4399,13 +4402,13 @@
         <v>19</v>
       </c>
       <c r="O16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AA16" t="s">
         <v>19</v>
       </c>
       <c r="AB16" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -4413,13 +4416,13 @@
         <v>20</v>
       </c>
       <c r="O17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AA17" t="s">
         <v>20</v>
       </c>
       <c r="AB17" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -4427,13 +4430,13 @@
         <v>21</v>
       </c>
       <c r="O18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AA18" t="s">
         <v>21</v>
       </c>
       <c r="AB18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -4441,13 +4444,13 @@
         <v>22</v>
       </c>
       <c r="O19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AA19" t="s">
         <v>22</v>
       </c>
       <c r="AB19" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -4458,7 +4461,7 @@
         <v>23</v>
       </c>
       <c r="AB20" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -4466,38 +4469,38 @@
         <v>31</v>
       </c>
       <c r="AB21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB22" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB23" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB24" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="AB26" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -4523,7 +4526,7 @@
         <v>81</v>
       </c>
       <c r="AB27" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -4549,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="AB28" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -4575,7 +4578,7 @@
         <v>43</v>
       </c>
       <c r="AB29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -4592,7 +4595,7 @@
         <v>44</v>
       </c>
       <c r="AB30" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -4603,7 +4606,7 @@
         <v>45</v>
       </c>
       <c r="AB31" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -4611,7 +4614,7 @@
         <v>46</v>
       </c>
       <c r="AB32" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="7:28" x14ac:dyDescent="0.25">
@@ -4619,7 +4622,7 @@
         <v>47</v>
       </c>
       <c r="AB33" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="7:28" x14ac:dyDescent="0.25">
@@ -4627,7 +4630,7 @@
         <v>48</v>
       </c>
       <c r="AB34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="7:28" x14ac:dyDescent="0.25">
@@ -4635,7 +4638,7 @@
         <v>49</v>
       </c>
       <c r="AB35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="7:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Flex Course -> FlexCourse
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE922F-3827-4A31-840C-0935DD72D4EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123C0F9-CC37-4282-BCA2-4D03F024355A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="467">
   <si>
     <t>course_code</t>
   </si>
@@ -1220,9 +1220,6 @@
   </si>
   <si>
     <t>If ECON 0110 is exempted, you must take an additional 1000-level Econ class</t>
-  </si>
-  <si>
-    <t>Flex Course</t>
   </si>
   <si>
     <t>APMA 0330 and APMA 0340 will sometimes be accepted in place of APMA 0350 and APMA 0360</t>
@@ -1942,10 +1939,10 @@
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="T3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2007,10 +2004,10 @@
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="T4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -2021,7 +2018,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2072,10 +2069,10 @@
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="T5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -2137,10 +2134,10 @@
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="T6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -2151,7 +2148,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2202,10 +2199,10 @@
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="T7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -2267,10 +2264,10 @@
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="T8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -2281,7 +2278,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2332,10 +2329,10 @@
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="T9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -2397,10 +2394,10 @@
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="T10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -2462,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="T11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -2527,10 +2524,10 @@
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="T12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -2592,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2657,10 +2654,10 @@
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2722,10 +2719,10 @@
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -2787,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -2852,10 +2849,10 @@
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -2917,10 +2914,10 @@
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -2982,10 +2979,10 @@
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="T19" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -3047,10 +3044,10 @@
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="T20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -3112,10 +3109,10 @@
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -3177,10 +3174,10 @@
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T22" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -3242,10 +3239,10 @@
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="T23" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -3298,10 +3295,10 @@
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="T24" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -3354,10 +3351,10 @@
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -3410,10 +3407,10 @@
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -3466,10 +3463,10 @@
         <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="T27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -3522,10 +3519,10 @@
         <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -3560,10 +3557,10 @@
         <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3598,10 +3595,10 @@
         <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="U30">
         <v>0</v>
@@ -3636,10 +3633,10 @@
         <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -3674,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -3712,10 +3709,10 @@
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T33" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="U33">
         <v>0</v>
@@ -3750,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="T34" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -3978,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,13 +3999,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K2" t="s">
         <v>329</v>
       </c>
       <c r="V2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="W2" t="s">
         <v>335</v>
@@ -4070,7 +4067,7 @@
         <v>341</v>
       </c>
       <c r="AC3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AD3" t="s">
         <v>342</v>
@@ -4170,7 +4167,7 @@
         <v>155</v>
       </c>
       <c r="P5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="V5" t="s">
         <v>8</v>
@@ -4194,10 +4191,10 @@
         <v>256</v>
       </c>
       <c r="AC5" t="s">
+        <v>465</v>
+      </c>
+      <c r="AD5" t="s">
         <v>466</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -4247,7 +4244,7 @@
         <v>257</v>
       </c>
       <c r="AC6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -4270,7 +4267,7 @@
         <v>251</v>
       </c>
       <c r="X7" t="s">
-        <v>396</v>
+        <v>465</v>
       </c>
       <c r="AA7" t="s">
         <v>11</v>
@@ -4279,7 +4276,7 @@
         <v>258</v>
       </c>
       <c r="AC7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changing the major input now removes the major unless it is done through updatePickerInput
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123C0F9-CC37-4282-BCA2-4D03F024355A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2AE96B-B664-4B2D-9643-62A56885AD53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>course_code</t>
   </si>
   <si>
-    <t>math AB</t>
-  </si>
-  <si>
     <t>MATH 1140</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>MATH 0760</t>
   </si>
   <si>
-    <t>econ AB</t>
-  </si>
-  <si>
     <t>MATH 0170</t>
   </si>
   <si>
@@ -1021,9 +1015,6 @@
     <t>csciStartup</t>
   </si>
   <si>
-    <t>apma AB</t>
-  </si>
-  <si>
     <t>ODEs</t>
   </si>
   <si>
@@ -1039,9 +1030,6 @@
     <t>One couse to be approved</t>
   </si>
   <si>
-    <t>math-cs SCB</t>
-  </si>
-  <si>
     <t>Semester 1 Intro</t>
   </si>
   <si>
@@ -1433,6 +1421,18 @@
   </si>
   <si>
     <t xml:space="preserve">Capstone </t>
+  </si>
+  <si>
+    <t>Apma AB</t>
+  </si>
+  <si>
+    <t>Math-CS ScB</t>
+  </si>
+  <si>
+    <t>Math AB</t>
+  </si>
+  <si>
+    <t>Econ AB</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1885,64 +1885,64 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="Q3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="T3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1950,64 +1950,64 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="Q4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="T4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -2015,64 +2015,64 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="Q5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="T5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -2080,64 +2080,64 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="Q6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="T6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -2145,64 +2145,64 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="Q7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="T7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -2210,64 +2210,64 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="Q8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="T8" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -2275,64 +2275,64 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="Q9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="T9" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -2340,64 +2340,64 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="Q10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="T10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -2405,64 +2405,64 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="Q11" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="T11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -2470,64 +2470,64 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="Q12" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="T12" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -2535,64 +2535,64 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q13" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="T13" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2600,64 +2600,64 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="Q14" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="T14" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2665,64 +2665,64 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Q15" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="T15" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -2730,64 +2730,64 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="Q16" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="T16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -2795,64 +2795,64 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="Q17" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="T17" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -2860,64 +2860,64 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="Q18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="T18" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -2925,64 +2925,64 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="N19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="Q19" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="T19" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -2990,64 +2990,64 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="Q20" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="T20" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -3055,64 +3055,64 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="Q21" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="T21" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -3120,64 +3120,64 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N22" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="Q22" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="T22" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -3185,64 +3185,64 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="Q23" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="T23" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -3250,55 +3250,55 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="Q24" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="T24" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -3306,55 +3306,55 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="Q25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="T25" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -3362,55 +3362,55 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="Q26" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="T26" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -3418,55 +3418,55 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K27" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="Q27" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="T27" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -3474,55 +3474,55 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="Q28" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="T28" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -3530,37 +3530,37 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N29" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="T29" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3568,37 +3568,37 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N30" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="T30" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="U30">
         <v>0</v>
@@ -3606,37 +3606,37 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="T31" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -3644,37 +3644,37 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N32" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="T32" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -3682,37 +3682,37 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="N33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="T33" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="U33">
         <v>0</v>
@@ -3720,37 +3720,37 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="T34" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -3758,19 +3758,19 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="N35" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -3781,19 +3781,19 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N36" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -3801,19 +3801,19 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N37" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -3821,19 +3821,19 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="N38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -3841,19 +3841,19 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N39" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -3861,19 +3861,19 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N40" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -3881,19 +3881,19 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N41" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -3901,10 +3901,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N42" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -3912,10 +3912,10 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -3923,10 +3923,10 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N44" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -3934,10 +3934,10 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N45" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -3945,10 +3945,10 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N46" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -3956,10 +3956,10 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N47" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -3975,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,84 +3993,84 @@
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>465</v>
       </c>
       <c r="J2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="K2" t="s">
-        <v>329</v>
+        <v>463</v>
       </c>
       <c r="V2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="W2" t="s">
-        <v>335</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
       <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" t="s">
+        <v>327</v>
+      </c>
+      <c r="M3" t="s">
+        <v>328</v>
+      </c>
+      <c r="N3" t="s">
+        <v>329</v>
+      </c>
+      <c r="O3" t="s">
+        <v>330</v>
+      </c>
+      <c r="P3" t="s">
+        <v>331</v>
+      </c>
+      <c r="V3" t="s">
         <v>71</v>
       </c>
-      <c r="K3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" t="s">
-        <v>330</v>
-      </c>
-      <c r="M3" t="s">
-        <v>331</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="W3" t="s">
         <v>332</v>
       </c>
-      <c r="O3" t="s">
+      <c r="X3" t="s">
         <v>333</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Y3" t="s">
         <v>334</v>
       </c>
-      <c r="V3" t="s">
-        <v>73</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA3" t="s">
         <v>336</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AB3" t="s">
         <v>337</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AC3" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD3" t="s">
         <v>338</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>339</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>340</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>341</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>398</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -4137,393 +4137,393 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M5" t="s">
+        <v>151</v>
+      </c>
+      <c r="N5" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" t="s">
         <v>153</v>
       </c>
-      <c r="N5" t="s">
-        <v>149</v>
-      </c>
-      <c r="O5" t="s">
-        <v>155</v>
-      </c>
       <c r="P5" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="V5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" t="s">
+        <v>245</v>
+      </c>
+      <c r="X5" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA5" t="s">
         <v>8</v>
       </c>
-      <c r="W5" t="s">
-        <v>247</v>
-      </c>
-      <c r="X5" t="s">
-        <v>248</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>253</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>9</v>
-      </c>
       <c r="AB5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AC5" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AD5" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="W6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="X6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="Y6" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z6" t="s">
         <v>254</v>
       </c>
-      <c r="Z6" t="s">
-        <v>256</v>
-      </c>
       <c r="AA6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AC6" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="W7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="X7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AA7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AC7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AA8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AA9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AA10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AA11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AA12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AB13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AB14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AA15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AA16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AA17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB17" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AA18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AB18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AA19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AB19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>466</v>
       </c>
       <c r="AB26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>77</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>79</v>
       </c>
-      <c r="F27" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" t="s">
-        <v>81</v>
-      </c>
       <c r="AB27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -4549,198 +4549,198 @@
         <v>5</v>
       </c>
       <c r="AB28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
         <v>39</v>
       </c>
-      <c r="E29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>41</v>
       </c>
-      <c r="G29" t="s">
-        <v>43</v>
-      </c>
       <c r="AB29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" t="s">
         <v>42</v>
       </c>
-      <c r="G30" t="s">
-        <v>44</v>
-      </c>
       <c r="AB30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AB31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AB32" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AB33" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AB34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AB35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data, updated code and helpers
</commit_message>
<xml_diff>
--- a/data/provided/Department Courses.xlsx
+++ b/data/provided/Department Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\shiny_personal\course_planner\data\provided\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2AE96B-B664-4B2D-9643-62A56885AD53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CA0CB2-B311-4184-9223-C898649C95DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E601DBE6-96E0-4FE1-9F7C-E0164527EEA9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="599">
   <si>
     <t>course_code</t>
   </si>
@@ -1433,6 +1433,402 @@
   </si>
   <si>
     <t>Econ AB</t>
+  </si>
+  <si>
+    <t>Behavioral Decision Sciences AB</t>
+  </si>
+  <si>
+    <t>Making Decisions</t>
+  </si>
+  <si>
+    <t>CLPS 0220</t>
+  </si>
+  <si>
+    <t>Choose One</t>
+  </si>
+  <si>
+    <t>CLPS 0400</t>
+  </si>
+  <si>
+    <t>CLPS 0200</t>
+  </si>
+  <si>
+    <t>CLPS 0700</t>
+  </si>
+  <si>
+    <t>Choose Two</t>
+  </si>
+  <si>
+    <t>CLPS 1470</t>
+  </si>
+  <si>
+    <t>CLPS 1495</t>
+  </si>
+  <si>
+    <t>CLPS 1730</t>
+  </si>
+  <si>
+    <t>CLPS 1760</t>
+  </si>
+  <si>
+    <t>One Introductory Course</t>
+  </si>
+  <si>
+    <t>Two Advanced Courses</t>
+  </si>
+  <si>
+    <t>ECON 1660</t>
+  </si>
+  <si>
+    <t>PHIL 0580</t>
+  </si>
+  <si>
+    <t>PHIL 1550</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>CLPS 0900</t>
+  </si>
+  <si>
+    <t>CLPS 1791</t>
+  </si>
+  <si>
+    <t>PHIL 0540</t>
+  </si>
+  <si>
+    <t>Three Electives</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>CLPS 0950</t>
+  </si>
+  <si>
+    <t>CLPS 1292</t>
+  </si>
+  <si>
+    <t>CLPS 1370</t>
+  </si>
+  <si>
+    <t>CLPS 1970</t>
+  </si>
+  <si>
+    <t>APMA 0200</t>
+  </si>
+  <si>
+    <t>APMA 2640</t>
+  </si>
+  <si>
+    <t>APMA 2821V</t>
+  </si>
+  <si>
+    <t>PHIL 0500</t>
+  </si>
+  <si>
+    <t>PHIL 1650</t>
+  </si>
+  <si>
+    <t>PHIL 1750</t>
+  </si>
+  <si>
+    <t>CSCI 1951A</t>
+  </si>
+  <si>
+    <t>POLS 1090</t>
+  </si>
+  <si>
+    <t>POLS 1150</t>
+  </si>
+  <si>
+    <t>POLS 1470</t>
+  </si>
+  <si>
+    <t>PHP 1740</t>
+  </si>
+  <si>
+    <t>Capstone</t>
+  </si>
+  <si>
+    <t>The Electives list suggested courses. Other custom courses can be taken and all must be approved by a concentration advisor</t>
+  </si>
+  <si>
+    <t>CLPS 0010</t>
+  </si>
+  <si>
+    <t>CLPS 0050A</t>
+  </si>
+  <si>
+    <t>CLPS 0100</t>
+  </si>
+  <si>
+    <t>CLPS 0120</t>
+  </si>
+  <si>
+    <t>CLPS 0300</t>
+  </si>
+  <si>
+    <t>CLPS 0500</t>
+  </si>
+  <si>
+    <t>CLPS 0540</t>
+  </si>
+  <si>
+    <t>CLPS 0550</t>
+  </si>
+  <si>
+    <t>CLPS 0610</t>
+  </si>
+  <si>
+    <t>CLPS 0611</t>
+  </si>
+  <si>
+    <t>CLPS 0701</t>
+  </si>
+  <si>
+    <t>CLPS 0800</t>
+  </si>
+  <si>
+    <t>CLPS 1181A</t>
+  </si>
+  <si>
+    <t>CLPS 1191</t>
+  </si>
+  <si>
+    <t>CLPS 1193</t>
+  </si>
+  <si>
+    <t>CLPS 1194</t>
+  </si>
+  <si>
+    <t>CLPS 1195</t>
+  </si>
+  <si>
+    <t>CLPS 1250</t>
+  </si>
+  <si>
+    <t>CLPS 1280B</t>
+  </si>
+  <si>
+    <t>CLPS 1310</t>
+  </si>
+  <si>
+    <t>CLPS 1331</t>
+  </si>
+  <si>
+    <t>CLPS 1342</t>
+  </si>
+  <si>
+    <t>CLPS 1478</t>
+  </si>
+  <si>
+    <t>CLPS 1480C</t>
+  </si>
+  <si>
+    <t>CLPS 1492</t>
+  </si>
+  <si>
+    <t>CLPS 1500</t>
+  </si>
+  <si>
+    <t>CLPS 1510</t>
+  </si>
+  <si>
+    <t>CLPS 1570</t>
+  </si>
+  <si>
+    <t>CLPS 1580C</t>
+  </si>
+  <si>
+    <t>CLPS 1590</t>
+  </si>
+  <si>
+    <t>CLPS 1610</t>
+  </si>
+  <si>
+    <t>CLPS 1620</t>
+  </si>
+  <si>
+    <t>CLPS 1660</t>
+  </si>
+  <si>
+    <t>CLPS 1700</t>
+  </si>
+  <si>
+    <t>CLPS 1720</t>
+  </si>
+  <si>
+    <t>CLPS 1770</t>
+  </si>
+  <si>
+    <t>CLPS 1782</t>
+  </si>
+  <si>
+    <t>CLPS 1790</t>
+  </si>
+  <si>
+    <t>CLPS 1890</t>
+  </si>
+  <si>
+    <t>CLPS 1900</t>
+  </si>
+  <si>
+    <t>CLPS 1960</t>
+  </si>
+  <si>
+    <t>Mind, Brain and Behavior: An Interdisciplinary Approach</t>
+  </si>
+  <si>
+    <t>Computing as Done in Brains and Computers</t>
+  </si>
+  <si>
+    <t>Learning and Conditioning</t>
+  </si>
+  <si>
+    <t>Introduction to Sleep</t>
+  </si>
+  <si>
+    <t>Human Cognition</t>
+  </si>
+  <si>
+    <t>Introduction to Linguistics</t>
+  </si>
+  <si>
+    <t>Cognitive Neuroscience</t>
+  </si>
+  <si>
+    <t>Perception and Mind</t>
+  </si>
+  <si>
+    <t>Simulating Reality: The (Curious) History and Science of Immersive Experiences</t>
+  </si>
+  <si>
+    <t>Science of Consciousness</t>
+  </si>
+  <si>
+    <t>Children's Thinking: The Nature of Cognitive Development</t>
+  </si>
+  <si>
+    <t>Children's Thinking</t>
+  </si>
+  <si>
+    <t>Social Psychology</t>
+  </si>
+  <si>
+    <t>Personality</t>
+  </si>
+  <si>
+    <t>Language and the Mind</t>
+  </si>
+  <si>
+    <t>Statistical Methods</t>
+  </si>
+  <si>
+    <t>Introduction to Programming</t>
+  </si>
+  <si>
+    <t>Canine Behavior (ONLINE)</t>
+  </si>
+  <si>
+    <t>Animal Behavior Laboratory</t>
+  </si>
+  <si>
+    <t>Laboratory in Genes and Behavior</t>
+  </si>
+  <si>
+    <t>Sleep and Chronobiology Research</t>
+  </si>
+  <si>
+    <t>Life Under Waer in the Anthropocene</t>
+  </si>
+  <si>
+    <t>Human Factors</t>
+  </si>
+  <si>
+    <t>Special Topics in Cognition: Collective Cognition</t>
+  </si>
+  <si>
+    <t>Phonology</t>
+  </si>
+  <si>
+    <t>Linguistic Variation and Universals</t>
+  </si>
+  <si>
+    <t>Compositional Semantics</t>
+  </si>
+  <si>
+    <t>Pragmatics</t>
+  </si>
+  <si>
+    <t>Translational Models of Neuropsychiatric Disorder</t>
+  </si>
+  <si>
+    <t>Cognitive Control Functions of the Prefrontal Cortex</t>
+  </si>
+  <si>
+    <t>Computational Cognitive Neuroscience</t>
+  </si>
+  <si>
+    <t>Affective Neuroscience</t>
+  </si>
+  <si>
+    <t>Perception and Action</t>
+  </si>
+  <si>
+    <t>Auditory Perception Laboratory</t>
+  </si>
+  <si>
+    <t>Perceptual Learning</t>
+  </si>
+  <si>
+    <t>Visualizing Information</t>
+  </si>
+  <si>
+    <t>Visualizing Vision</t>
+  </si>
+  <si>
+    <t>Cognitive Development</t>
+  </si>
+  <si>
+    <t>Developmental Cognitive Neuroscience</t>
+  </si>
+  <si>
+    <t>Learning Compositional Language</t>
+  </si>
+  <si>
+    <t>Abnormal Psychology</t>
+  </si>
+  <si>
+    <t>Human Resilience</t>
+  </si>
+  <si>
+    <t>Psychology in Business and Economics</t>
+  </si>
+  <si>
+    <t>The Moral Brain</t>
+  </si>
+  <si>
+    <t>Stigma and Prejudice</t>
+  </si>
+  <si>
+    <t>Me, Myself, and I: Exploring Senses of Self from a Multidisciplinary Perspective (COST 1082)</t>
+  </si>
+  <si>
+    <t>Personality and Clinical Assessment</t>
+  </si>
+  <si>
+    <t>Laboratory in Social Cognition</t>
+  </si>
+  <si>
+    <t>Laboratory in Psycholingustics</t>
+  </si>
+  <si>
+    <t>Research Methods And Design</t>
+  </si>
+  <si>
+    <t>Senior Seminar in Behavioral Decision Sciences</t>
   </si>
 </sst>
 </file>
@@ -1793,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FF0174-35EF-4838-880B-C4F8D4E4CC9D}">
-  <dimension ref="A2:U47"/>
+  <dimension ref="A2:X54"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showZeros="0" topLeftCell="O5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,9 +2212,11 @@
     <col min="17" max="17" width="13.5703125" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" customWidth="1"/>
     <col min="20" max="20" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1882,8 +2280,14 @@
       <c r="U2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1947,8 +2351,17 @@
       <c r="U3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>507</v>
+      </c>
+      <c r="W3" t="s">
+        <v>548</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2012,8 +2425,17 @@
       <c r="U4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" t="s">
+        <v>508</v>
+      </c>
+      <c r="W4" t="s">
+        <v>549</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2077,8 +2499,17 @@
       <c r="U5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>509</v>
+      </c>
+      <c r="W5" t="s">
+        <v>550</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2142,8 +2573,17 @@
       <c r="U6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>510</v>
+      </c>
+      <c r="W6" t="s">
+        <v>551</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2207,8 +2647,17 @@
       <c r="U7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>472</v>
+      </c>
+      <c r="W7" t="s">
+        <v>552</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2272,8 +2721,17 @@
       <c r="U8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>469</v>
+      </c>
+      <c r="W8" t="s">
+        <v>468</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2337,8 +2795,17 @@
       <c r="U9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>511</v>
+      </c>
+      <c r="W9" t="s">
+        <v>553</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2402,8 +2869,17 @@
       <c r="U10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>471</v>
+      </c>
+      <c r="W10" t="s">
+        <v>554</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2467,8 +2943,17 @@
       <c r="U11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" t="s">
+        <v>512</v>
+      </c>
+      <c r="W11" t="s">
+        <v>555</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2532,8 +3017,17 @@
       <c r="U12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>513</v>
+      </c>
+      <c r="W12" t="s">
+        <v>556</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2597,8 +3091,17 @@
       <c r="U13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>514</v>
+      </c>
+      <c r="W13" t="s">
+        <v>557</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2662,8 +3165,17 @@
       <c r="U14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>515</v>
+      </c>
+      <c r="W14" t="s">
+        <v>558</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2727,8 +3239,17 @@
       <c r="U15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>516</v>
+      </c>
+      <c r="W15" t="s">
+        <v>559</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2792,8 +3313,17 @@
       <c r="U16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>473</v>
+      </c>
+      <c r="W16" t="s">
+        <v>560</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2857,8 +3387,17 @@
       <c r="U17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>517</v>
+      </c>
+      <c r="W17" t="s">
+        <v>561</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2922,8 +3461,17 @@
       <c r="U18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>518</v>
+      </c>
+      <c r="W18" t="s">
+        <v>562</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2987,8 +3535,17 @@
       <c r="U19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
+        <v>485</v>
+      </c>
+      <c r="W19" t="s">
+        <v>563</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3052,8 +3609,17 @@
       <c r="U20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>490</v>
+      </c>
+      <c r="W20" t="s">
+        <v>564</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3117,8 +3683,17 @@
       <c r="U21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>519</v>
+      </c>
+      <c r="W21" t="s">
+        <v>565</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3182,8 +3757,17 @@
       <c r="U22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>520</v>
+      </c>
+      <c r="W22" t="s">
+        <v>566</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3247,8 +3831,17 @@
       <c r="U23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>521</v>
+      </c>
+      <c r="W23" t="s">
+        <v>567</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3303,8 +3896,17 @@
       <c r="U24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>522</v>
+      </c>
+      <c r="W24" t="s">
+        <v>568</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -3359,8 +3961,17 @@
       <c r="U25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>523</v>
+      </c>
+      <c r="W25" t="s">
+        <v>569</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -3415,8 +4026,17 @@
       <c r="U26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>524</v>
+      </c>
+      <c r="W26" t="s">
+        <v>570</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3471,8 +4091,17 @@
       <c r="U27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>525</v>
+      </c>
+      <c r="W27" t="s">
+        <v>571</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -3527,8 +4156,17 @@
       <c r="U28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>526</v>
+      </c>
+      <c r="W28" t="s">
+        <v>572</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -3565,8 +4203,17 @@
       <c r="U29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>527</v>
+      </c>
+      <c r="W29" t="s">
+        <v>573</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3603,8 +4250,17 @@
       <c r="U30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>528</v>
+      </c>
+      <c r="W30" t="s">
+        <v>574</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3641,8 +4297,17 @@
       <c r="U31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>492</v>
+      </c>
+      <c r="W31" t="s">
+        <v>575</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -3679,8 +4344,17 @@
       <c r="U32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>529</v>
+      </c>
+      <c r="W32" t="s">
+        <v>576</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -3717,8 +4391,17 @@
       <c r="U33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>530</v>
+      </c>
+      <c r="W33" t="s">
+        <v>577</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -3755,8 +4438,17 @@
       <c r="U34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V34" t="s">
+        <v>531</v>
+      </c>
+      <c r="W34" t="s">
+        <v>578</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>62</v>
       </c>
@@ -3778,8 +4470,17 @@
       <c r="U35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>476</v>
+      </c>
+      <c r="W35" t="s">
+        <v>579</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>63</v>
       </c>
@@ -3798,8 +4499,17 @@
       <c r="O36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>532</v>
+      </c>
+      <c r="W36" t="s">
+        <v>580</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>64</v>
       </c>
@@ -3818,8 +4528,17 @@
       <c r="O37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>533</v>
+      </c>
+      <c r="W37" t="s">
+        <v>581</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>65</v>
       </c>
@@ -3838,8 +4557,17 @@
       <c r="O38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V38" t="s">
+        <v>534</v>
+      </c>
+      <c r="W38" t="s">
+        <v>582</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>66</v>
       </c>
@@ -3858,8 +4586,17 @@
       <c r="O39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V39" t="s">
+        <v>535</v>
+      </c>
+      <c r="W39" t="s">
+        <v>583</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>67</v>
       </c>
@@ -3878,8 +4615,17 @@
       <c r="O40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>536</v>
+      </c>
+      <c r="W40" t="s">
+        <v>584</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>68</v>
       </c>
@@ -3898,8 +4644,17 @@
       <c r="O41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V41" t="s">
+        <v>537</v>
+      </c>
+      <c r="W41" t="s">
+        <v>585</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
         <v>277</v>
       </c>
@@ -3909,8 +4664,17 @@
       <c r="O42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>538</v>
+      </c>
+      <c r="W42" t="s">
+        <v>586</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
         <v>278</v>
       </c>
@@ -3920,8 +4684,17 @@
       <c r="O43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>539</v>
+      </c>
+      <c r="W43" t="s">
+        <v>587</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
         <v>279</v>
       </c>
@@ -3931,8 +4704,17 @@
       <c r="O44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>540</v>
+      </c>
+      <c r="W44" t="s">
+        <v>588</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
         <v>280</v>
       </c>
@@ -3942,8 +4724,17 @@
       <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V45" t="s">
+        <v>541</v>
+      </c>
+      <c r="W45" t="s">
+        <v>589</v>
+      </c>
+      <c r="X45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
         <v>281</v>
       </c>
@@ -3953,8 +4744,17 @@
       <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>477</v>
+      </c>
+      <c r="W46" t="s">
+        <v>590</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
         <v>282</v>
       </c>
@@ -3962,6 +4762,92 @@
         <v>326</v>
       </c>
       <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="V47" t="s">
+        <v>478</v>
+      </c>
+      <c r="W47" t="s">
+        <v>591</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>542</v>
+      </c>
+      <c r="W48" t="s">
+        <v>592</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>543</v>
+      </c>
+      <c r="W49" t="s">
+        <v>593</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>544</v>
+      </c>
+      <c r="W50" t="s">
+        <v>594</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V51" t="s">
+        <v>486</v>
+      </c>
+      <c r="W51" t="s">
+        <v>595</v>
+      </c>
+      <c r="X51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>545</v>
+      </c>
+      <c r="W52" t="s">
+        <v>596</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V53" t="s">
+        <v>546</v>
+      </c>
+      <c r="W53" t="s">
+        <v>597</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="22:24" x14ac:dyDescent="0.25">
+      <c r="V54" t="s">
+        <v>547</v>
+      </c>
+      <c r="W54" t="s">
+        <v>598</v>
+      </c>
+      <c r="X54">
         <v>0</v>
       </c>
     </row>
@@ -3975,8 +4861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96243044-DAFC-4DB6-9967-18D55104159C}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4496,6 +5382,12 @@
       <c r="B26" t="s">
         <v>466</v>
       </c>
+      <c r="L26" t="s">
+        <v>506</v>
+      </c>
+      <c r="M26" t="s">
+        <v>467</v>
+      </c>
       <c r="AB26" t="s">
         <v>275</v>
       </c>
@@ -4522,6 +5414,33 @@
       <c r="G27" t="s">
         <v>79</v>
       </c>
+      <c r="L27" t="s">
+        <v>468</v>
+      </c>
+      <c r="M27" t="s">
+        <v>470</v>
+      </c>
+      <c r="N27" t="s">
+        <v>474</v>
+      </c>
+      <c r="O27" t="s">
+        <v>479</v>
+      </c>
+      <c r="P27" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>484</v>
+      </c>
+      <c r="R27" t="s">
+        <v>470</v>
+      </c>
+      <c r="S27" t="s">
+        <v>488</v>
+      </c>
+      <c r="T27" t="s">
+        <v>505</v>
+      </c>
       <c r="AB27" t="s">
         <v>276</v>
       </c>
@@ -4548,6 +5467,33 @@
       <c r="G28">
         <v>5</v>
       </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>3</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
       <c r="AB28" t="s">
         <v>277</v>
       </c>
@@ -4574,6 +5520,33 @@
       <c r="G29" t="s">
         <v>41</v>
       </c>
+      <c r="L29" t="s">
+        <v>469</v>
+      </c>
+      <c r="M29" t="s">
+        <v>471</v>
+      </c>
+      <c r="N29" t="s">
+        <v>475</v>
+      </c>
+      <c r="O29" t="s">
+        <v>34</v>
+      </c>
+      <c r="P29" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>152</v>
+      </c>
+      <c r="R29" t="s">
+        <v>486</v>
+      </c>
+      <c r="S29" t="s">
+        <v>489</v>
+      </c>
+      <c r="T29" t="s">
+        <v>505</v>
+      </c>
       <c r="AB29" t="s">
         <v>278</v>
       </c>
@@ -4591,6 +5564,27 @@
       <c r="G30" t="s">
         <v>42</v>
       </c>
+      <c r="M30" t="s">
+        <v>472</v>
+      </c>
+      <c r="N30" t="s">
+        <v>476</v>
+      </c>
+      <c r="O30" t="s">
+        <v>241</v>
+      </c>
+      <c r="P30" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>162</v>
+      </c>
+      <c r="R30" t="s">
+        <v>245</v>
+      </c>
+      <c r="S30" t="s">
+        <v>490</v>
+      </c>
       <c r="AB30" t="s">
         <v>279</v>
       </c>
@@ -4602,6 +5596,27 @@
       <c r="G31" t="s">
         <v>43</v>
       </c>
+      <c r="M31" t="s">
+        <v>473</v>
+      </c>
+      <c r="N31" t="s">
+        <v>477</v>
+      </c>
+      <c r="O31" t="s">
+        <v>245</v>
+      </c>
+      <c r="P31" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>485</v>
+      </c>
+      <c r="R31" t="s">
+        <v>247</v>
+      </c>
+      <c r="S31" t="s">
+        <v>491</v>
+      </c>
       <c r="AB31" t="s">
         <v>280</v>
       </c>
@@ -4610,6 +5625,24 @@
       <c r="G32" t="s">
         <v>44</v>
       </c>
+      <c r="N32" t="s">
+        <v>478</v>
+      </c>
+      <c r="O32" t="s">
+        <v>247</v>
+      </c>
+      <c r="P32" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>242</v>
+      </c>
+      <c r="R32" t="s">
+        <v>39</v>
+      </c>
+      <c r="S32" t="s">
+        <v>492</v>
+      </c>
       <c r="AB32" t="s">
         <v>281</v>
       </c>
@@ -4618,6 +5651,21 @@
       <c r="G33" t="s">
         <v>45</v>
       </c>
+      <c r="O33" t="s">
+        <v>248</v>
+      </c>
+      <c r="P33" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>267</v>
+      </c>
+      <c r="R33" t="s">
+        <v>40</v>
+      </c>
+      <c r="S33" t="s">
+        <v>493</v>
+      </c>
       <c r="AB33" t="s">
         <v>282</v>
       </c>
@@ -4626,6 +5674,21 @@
       <c r="G34" t="s">
         <v>46</v>
       </c>
+      <c r="O34" t="s">
+        <v>249</v>
+      </c>
+      <c r="P34" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R34" t="s">
+        <v>487</v>
+      </c>
+      <c r="S34" t="s">
+        <v>65</v>
+      </c>
       <c r="AB34" t="s">
         <v>162</v>
       </c>
@@ -4634,6 +5697,12 @@
       <c r="G35" t="s">
         <v>47</v>
       </c>
+      <c r="P35" t="s">
+        <v>68</v>
+      </c>
+      <c r="S35" t="s">
+        <v>68</v>
+      </c>
       <c r="AB35" t="s">
         <v>163</v>
       </c>
@@ -4642,103 +5711,151 @@
       <c r="G36" t="s">
         <v>48</v>
       </c>
+      <c r="P36" t="s">
+        <v>482</v>
+      </c>
+      <c r="S36" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="37" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>49</v>
       </c>
+      <c r="P37" t="s">
+        <v>483</v>
+      </c>
+      <c r="S37" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="38" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
         <v>50</v>
       </c>
+      <c r="S38" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="39" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
         <v>51</v>
       </c>
+      <c r="S39" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="40" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
         <v>52</v>
       </c>
+      <c r="S40" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="41" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
         <v>53</v>
       </c>
+      <c r="S41" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="42" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>54</v>
       </c>
+      <c r="S42" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="43" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>55</v>
       </c>
+      <c r="S43" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="44" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>56</v>
       </c>
+      <c r="S44" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>57</v>
       </c>
+      <c r="S45" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="46" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>58</v>
       </c>
+      <c r="S46" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="47" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>59</v>
       </c>
+      <c r="S47" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="48" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="S48" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="49" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="S49" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="50" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>68</v>
       </c>

</xml_diff>